<commit_message>
Tested and Commented parks_visitors_v_population.ipynb - note it correctly includes parks that span multiple states
</commit_message>
<xml_diff>
--- a/Resources/current_gas_prices.xlsx
+++ b/Resources/current_gas_prices.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annmcnamara/Desktop/National_Park_Analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFDDB2DF-CAB7-3340-9F40-CC10A52E8EB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E27EF2-32D1-5D44-9F9C-2EE6ED771A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{749AE98A-BCA1-9B46-B97D-DE7C30E5F57F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2019" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>State </t>
   </si>
@@ -184,13 +185,43 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Last Year</t>
+  </si>
+  <si>
+    <t>CA    3.676462</t>
+  </si>
+  <si>
+    <t>CO    2.686462</t>
+  </si>
+  <si>
+    <t>FL    2.522385</t>
+  </si>
+  <si>
+    <t>MA    2.667154</t>
+  </si>
+  <si>
+    <t>MN    2.512769</t>
+  </si>
+  <si>
+    <t>NY    2.731385</t>
+  </si>
+  <si>
+    <t>OH    2.561000</t>
+  </si>
+  <si>
+    <t>TX    2.360154</t>
+  </si>
+  <si>
+    <t>WA    3.178077</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -219,6 +250,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,11 +278,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="40" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -262,6 +301,1003 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.6764619999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6864620000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5223849999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.667154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.512769</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.731385</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3601540000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.178077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DABE-C748-A42B-B12B624759A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.282</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2810000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.913</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9670000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DABE-C748-A42B-B12B624759A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="728490015"/>
+        <c:axId val="671036415"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="728490015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671036415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="671036415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="728490015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0502B720-D8F8-5542-92E3-55BA11EDA770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,428 +1597,902 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1337B705-F70B-9849-8434-C7008B8F73E3}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I2" sqref="I2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="K1">
+        <v>2019</v>
+      </c>
+      <c r="L1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3">
         <v>2.8130000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F2" s="4">
+        <f>C2-D2</f>
+        <v>-2.8130000000000002</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2">
+        <v>3.6764619999999999</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3.282</v>
+      </c>
+      <c r="N2" s="4">
+        <f t="shared" ref="N2:N10" si="0">K2-L2</f>
+        <v>0.39446199999999987</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
         <v>1.9530000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F52" si="1">C3-D3</f>
+        <v>-1.9530000000000001</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
+        <v>2.6864620000000001</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2.1379999999999999</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.54846200000000023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3">
         <v>1.958</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.958</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
+        <v>2.5223849999999999</v>
+      </c>
+      <c r="L4" s="3">
+        <v>2.1190000000000002</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.40338499999999966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3">
         <v>2.633</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.633</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
+        <v>2.667154</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2.2810000000000001</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.38615399999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
+        <v>3.6764619999999999</v>
+      </c>
+      <c r="D6" s="3">
         <v>3.282</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.39446199999999987</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
+        <v>2.512769</v>
+      </c>
+      <c r="L6" s="3">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.4677690000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>2.6864620000000001</v>
+      </c>
+      <c r="D7" s="3">
         <v>2.1379999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.54846200000000023</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
+        <v>2.731385</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.28138499999999977</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
         <v>2.363</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.363</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
+        <v>2.5609999999999999</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1.881</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3">
         <v>2.4119999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.4119999999999999</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>2.3601540000000001</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.913</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.44715400000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3">
         <v>2.1070000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1070000000000002</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
+        <v>3.178077</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2.9670000000000001</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21107699999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
+        <v>2.5223849999999999</v>
+      </c>
+      <c r="D11" s="3">
         <v>2.1190000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40338499999999966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
         <v>2.0169999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.0169999999999999</v>
+      </c>
+      <c r="K12" t="e">
+        <f>regression</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N12" s="4">
+        <f>AVERAGE(N2:N10)</f>
+        <v>0.42442755555555556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3">
         <v>3.516</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.516</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3">
         <v>1.978</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3">
         <v>2.5110000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.5110000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="23" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3">
         <v>2.23</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3">
         <v>1.905</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.905</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3">
         <v>1.9510000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9510000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3">
         <v>1.911</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3">
         <v>1.9670000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F20" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9670000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
+        <v>2.667154</v>
+      </c>
+      <c r="D21" s="3">
         <v>2.2810000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38615399999999989</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3">
         <v>2.1920000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1920000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3">
         <v>2.14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3">
         <v>1.9379999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F24" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9379999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
+        <v>2.512769</v>
+      </c>
+      <c r="D25" s="3">
         <v>2.0449999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F25" s="4">
+        <f t="shared" si="1"/>
+        <v>0.4677690000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3">
         <v>1.921</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F26" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.921</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3">
         <v>1.9139999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F27" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9139999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3">
         <v>2.29</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F28" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F29" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3">
         <v>2.048</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F30" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.048</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3">
         <v>2.117</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F31" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3">
         <v>2.2360000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F32" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.2360000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3">
         <v>2.3260000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F33" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.3260000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="3">
         <v>2.1139999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F34" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1139999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="3">
         <v>2.7879999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F35" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.7879999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2">
+        <v>2.731385</v>
+      </c>
+      <c r="D36" s="3">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F36" s="4">
+        <f t="shared" si="1"/>
+        <v>0.28138499999999977</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
+        <v>2.5609999999999999</v>
+      </c>
+      <c r="D37" s="3">
         <v>1.881</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F37" s="4">
+        <f t="shared" si="1"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="3">
         <v>1.8380000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F38" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.8380000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3">
         <v>2.879</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F39" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3">
         <v>2.419</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F40" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.419</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3">
         <v>2.2989999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F41" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.2989999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3">
         <v>1.9219999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F42" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9219999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3">
         <v>2.1560000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F43" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1560000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3">
         <v>1.9690000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F44" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9690000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2">
+        <v>2.3601540000000001</v>
+      </c>
+      <c r="D45" s="3">
         <v>1.913</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F45" s="4">
+        <f t="shared" si="1"/>
+        <v>0.44715400000000005</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3">
         <v>2.4649999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F46" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.4649999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F47" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3">
         <v>2.347</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F48" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.347</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2">
+        <v>3.178077</v>
+      </c>
+      <c r="D49" s="3">
         <v>2.9670000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F49" s="4">
+        <f t="shared" si="1"/>
+        <v>0.21107699999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3">
         <v>1.9430000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F50" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.9430000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3">
         <v>2.1819999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+      <c r="F51" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.1819999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="23" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3">
         <v>2.3439999999999999</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.3439999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D55" s="4">
+        <f>AVERAGE(D2:D52)</f>
+        <v>2.2374117647058824</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +2548,82 @@
     <hyperlink ref="A50" r:id="rId49" display="https://gasprices.aaa.com/?state=WI" xr:uid="{5CF66A94-0746-3E40-B414-B0ED538B6ACC}"/>
     <hyperlink ref="A51" r:id="rId50" display="https://gasprices.aaa.com/?state=WV" xr:uid="{03AC0D70-B7A3-5F41-A000-8065F01B0892}"/>
     <hyperlink ref="A52" r:id="rId51" display="https://gasprices.aaa.com/?state=WY" xr:uid="{89D444EA-C254-F544-8C4D-90C875B4EFCE}"/>
+    <hyperlink ref="I2" r:id="rId52" display="https://gasprices.aaa.com/?state=CA" xr:uid="{B62C3219-8A6D-9F49-AF92-151BF67F582B}"/>
+    <hyperlink ref="I3" r:id="rId53" display="https://gasprices.aaa.com/?state=CO" xr:uid="{659DF590-0169-D34B-A5B1-03C3149647C4}"/>
+    <hyperlink ref="I4" r:id="rId54" display="https://gasprices.aaa.com/?state=FL" xr:uid="{5C9C9F42-E631-8740-8837-CCDF076E7230}"/>
+    <hyperlink ref="I5" r:id="rId55" display="https://gasprices.aaa.com/?state=MA" xr:uid="{631EAE7F-62A4-DA48-97C5-1F8D3A2BAA62}"/>
+    <hyperlink ref="I6" r:id="rId56" display="https://gasprices.aaa.com/?state=MN" xr:uid="{583A2A15-19AE-7E47-88E1-3597CCD8694A}"/>
+    <hyperlink ref="I7" r:id="rId57" display="https://gasprices.aaa.com/?state=NY" xr:uid="{D3036C8B-D0FE-A749-8930-419F9BDEDF30}"/>
+    <hyperlink ref="I8" r:id="rId58" display="https://gasprices.aaa.com/?state=OH" xr:uid="{D70D793A-CCDE-B843-A0C6-5B384778CA4D}"/>
+    <hyperlink ref="I9" r:id="rId59" display="https://gasprices.aaa.com/?state=TX" xr:uid="{54569803-C987-1245-8C97-E1ECD726F4F8}"/>
+    <hyperlink ref="I10" r:id="rId60" display="https://gasprices.aaa.com/?state=WA" xr:uid="{54AA9DAF-20B9-0C4B-B814-A2EEEA4B9526}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId61"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEC5C26-78C0-434A-94E5-7A0AE6F4A89F}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>